<commit_message>
Excel required bug fixed
</commit_message>
<xml_diff>
--- a/danaks_export_v1_0_0.xlsx
+++ b/danaks_export_v1_0_0.xlsx
@@ -488,19 +488,19 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Activity</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CardiacArrestWithin12h</t>
+          <t>CardiacRehabPlan</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr">
         <is>
-          <t>ResultValue</t>
+          <t>StatusCode</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -510,36 +510,36 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Cardiac arrest prehospital or within 12 hours after hospitalization.</t>
+          <t>Rehabilitation.</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | ja | nej | </t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>True</t>
+          <t xml:space="preserve">Enums/Udfald: | ja_patienten_accepterer | ja_patienten_afslaar | nej_ikke_relevant | </t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Diagnosis</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>AcuteHeartFailureKillipClass</t>
+          <t>VerifiedDiagnosis</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="D5" t="inlineStr">
         <is>
-          <t>ResultValue</t>
+          <t>DiagnosisType</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -549,12 +549,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Killip class within 12 hours after hospitalization.</t>
+          <t>Final diagnosis verified by cardiologist at discharge.</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | killip_klasse1 | killip_klasse2 | killip_klasse3 | killip_klasse4 | </t>
+          <t xml:space="preserve">Enums/Udfald: | di200 | di213a | di213b | di213c | di214 | ikke_aks | </t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -566,19 +566,24 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Contact</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CardiogenicShockAfter12h</t>
+          <t>AdmissionDate</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="D7" t="inlineStr">
         <is>
-          <t>ResultValue</t>
+          <t>DateTime</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -588,12 +593,12 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>CardiogenicShock later than 12 hours after hospitalization</t>
+          <t>Date and time for admission.</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | ja | nej | ikke_relevant | </t>
+          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -610,7 +615,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>LVEF</t>
+          <t>CardiacArrestWithin12h</t>
         </is>
       </c>
     </row>
@@ -622,22 +627,17 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>str</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>LVEF: Left ventricular ejection fraction.</t>
+          <t>Cardiac arrest prehospital or within 12 hours after hospitalization.</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 100</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>True</t>
+          <t xml:space="preserve">Enums/Udfald: | ja | nej | </t>
         </is>
       </c>
     </row>
@@ -649,7 +649,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>CardiacArrestAfter12h</t>
+          <t>AcuteHeartFailureKillipClass</t>
         </is>
       </c>
     </row>
@@ -666,17 +666,12 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Cardiogenic shock later than 12 hours after hospitalization.</t>
+          <t>Killip class within 12 hours after hospitalization.</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | ja | nej | ikke_relevant | </t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>True</t>
+          <t xml:space="preserve">Enums/Udfald: | killip_klasse1 | killip_klasse2 | killip_klasse3 | killip_klasse4 | </t>
         </is>
       </c>
     </row>
@@ -713,28 +708,23 @@
           <t xml:space="preserve">Enums/Udfald: | ja | nej | </t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Diagnosis</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>VerifiedDiagnosis</t>
+          <t>CardiacArrestAfter12h</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="D15" t="inlineStr">
         <is>
-          <t>DiagnosisType</t>
+          <t>ResultValue</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -744,36 +734,31 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Final diagnosis verified by cardiologist at discharge.</t>
+          <t>Cardiogenic shock later than 12 hours after hospitalization.</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | di200 | di213a | di213b | di213c | di214 | ikke_aks | </t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>True</t>
+          <t xml:space="preserve">Enums/Udfald: | ja | nej | ikke_relevant | </t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Contact</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>AdmissionDate</t>
+          <t>CardiogenicShockAfter12h</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="D17" t="inlineStr">
         <is>
-          <t>DateTime</t>
+          <t>ResultValue</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -783,56 +768,46 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Date and time for admission.</t>
+          <t>CardiogenicShock later than 12 hours after hospitalization</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>True</t>
+          <t xml:space="preserve">Enums/Udfald: | ja | nej | ikke_relevant | </t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Activity</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>CardiacRehabPlan</t>
+          <t>LVEF</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="D19" t="inlineStr">
         <is>
-          <t>StatusCode</t>
+          <t>ResultValue</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>int</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Rehabilitation.</t>
+          <t>LVEF: Left ventricular ejection fraction.</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | ja_patienten_accepterer | ja_patienten_afslaar | nej_ikke_relevant | </t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>True</t>
+          <t>Greater than or equal to: 0 | Less than or equal to: 100</t>
         </is>
       </c>
     </row>

</xml_diff>